<commit_message>
Add another formula for operators
</commit_message>
<xml_diff>
--- a/2_Formulas_and_Functions/1_Formulas_Intro/1_Formulas_Basics.xlsx
+++ b/2_Formulas_and_Functions/1_Formulas_Intro/1_Formulas_Basics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaderPC\Documents\GitHub\Excel_Data_Analytics_Course\2_Formulas_and_Functions\1_Formulas_Intro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8124C3B2-3F80-4F1F-83E7-D0DC5946D7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A2D3A2-FFAC-4980-B2B6-98DA261BD6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="2" r:id="rId1"/>
@@ -383,7 +383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54668AE6-8A31-4CB0-BFA9-581007C29CED}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,6 +544,12 @@
         <v>17</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>13-2+(15/3)^2</f>
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>